<commit_message>
Adjusted Directory and prepped for Heroku
</commit_message>
<xml_diff>
--- a/KlangValleyIsochroneAnalysis/resources/data/raw_data/klang_valley_stations.xlsx
+++ b/KlangValleyIsochroneAnalysis/resources/data/raw_data/klang_valley_stations.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="429">
   <si>
-    <t xml:space="preserve"> Stop Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Stop ID</t>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop ID</t>
   </si>
   <si>
     <t xml:space="preserve">Service Provider Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Latitud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitud</t>
+    <t xml:space="preserve">Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitude</t>
   </si>
   <si>
     <t xml:space="preserve">ROUTE ID</t>
@@ -1487,11 +1487,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Trains" displayName="Trains" ref="A1:J206" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:J206"/>
   <tableColumns count="10">
-    <tableColumn id="1" name=" Stop Name"/>
-    <tableColumn id="2" name=" Stop ID"/>
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Stop ID"/>
     <tableColumn id="3" name="Service Provider Name"/>
-    <tableColumn id="4" name="Latitud"/>
-    <tableColumn id="5" name="Longitud"/>
+    <tableColumn id="4" name="Latitude"/>
+    <tableColumn id="5" name="Longitude"/>
     <tableColumn id="6" name="ROUTE ID"/>
     <tableColumn id="7" name="Route Name"/>
     <tableColumn id="8" name="Line Number"/>
@@ -1509,7 +1509,7 @@
   <dimension ref="A1:L206"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2:K206"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>